<commit_message>
Updated ISA, still 8-bit, contemplating migration to 16-bit ISA for more flexibility.  CPyU.py program updated with load, add, subtract and logical and functions implemented.  No memory size check yet, needs to be implemented.  machine.a updated with simple program that loads values into three registers and performs a subtraction and a logical and function in order to test program functionality.
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>Op-code</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>nop</t>
+  </si>
+  <si>
+    <t>V = Has Return Value (True/False)</t>
   </si>
 </sst>
 </file>
@@ -397,13 +400,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,34 +428,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +764,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -760,42 +773,43 @@
     <col min="2" max="9" width="3.7109375" customWidth="1"/>
     <col min="10" max="10" width="3.85546875" customWidth="1"/>
     <col min="11" max="17" width="3.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>0</v>
       </c>
       <c r="C2" s="2">
@@ -804,27 +818,27 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
       <c r="C3" s="2">
@@ -833,27 +847,27 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>0</v>
       </c>
       <c r="C4" s="2">
@@ -862,19 +876,19 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
         <v>0</v>
       </c>
       <c r="K4" t="s">
@@ -882,31 +896,31 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13">
-        <v>0</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
         <v>0</v>
       </c>
       <c r="K5" t="s">
@@ -914,10 +928,10 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>0</v>
       </c>
       <c r="C6" s="2">
@@ -926,27 +940,30 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <v>1</v>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>0</v>
       </c>
       <c r="C7" s="2">
@@ -955,36 +972,36 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="9">
-        <v>1</v>
-      </c>
-      <c r="K7" s="18" t="s">
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="K7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>0</v>
       </c>
       <c r="C8" s="2">
@@ -993,34 +1010,34 @@
       <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>0</v>
       </c>
       <c r="C9" s="2">
@@ -1029,27 +1046,27 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="11">
         <v>0</v>
       </c>
       <c r="C10" s="2">
@@ -1058,27 +1075,27 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="11">
         <v>0</v>
       </c>
       <c r="C11" s="2">
@@ -1087,27 +1104,27 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <v>1</v>
       </c>
       <c r="C12" s="2">
@@ -1116,27 +1133,27 @@
       <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>1</v>
       </c>
       <c r="C13" s="2">
@@ -1145,27 +1162,27 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>1</v>
       </c>
       <c r="C14" s="2">
@@ -1174,27 +1191,27 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="9" t="s">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>1</v>
       </c>
       <c r="C15" s="2">
@@ -1203,27 +1220,27 @@
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>1</v>
       </c>
       <c r="C16" s="2">
@@ -1232,27 +1249,27 @@
       <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>1</v>
       </c>
       <c r="C17" s="2">
@@ -1261,27 +1278,27 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
       <c r="C18" s="2">
@@ -1290,27 +1307,27 @@
       <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>1</v>
       </c>
       <c r="C19" s="2">
@@ -1319,27 +1336,27 @@
       <c r="D19" s="2">
         <v>0</v>
       </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="8">
-        <v>1</v>
-      </c>
-      <c r="I19" s="9">
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="7">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>1</v>
       </c>
       <c r="C20" s="2">
@@ -1348,27 +1365,27 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="8">
-        <v>1</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>1</v>
       </c>
       <c r="C21" s="2">
@@ -1377,36 +1394,36 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0</v>
-      </c>
-      <c r="K21" s="18" t="s">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="11">
         <v>1</v>
       </c>
       <c r="C22" s="2">
@@ -1415,100 +1432,100 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="15">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="9">
-        <v>1</v>
-      </c>
-      <c r="H23" s="8">
-        <v>1</v>
-      </c>
-      <c r="I23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
+      <c r="B23" s="11">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8">
+        <v>1</v>
+      </c>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="15">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="9" t="s">
+      <c r="B24" s="11">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="21">
         <v>1</v>
@@ -1519,55 +1536,57 @@
       <c r="E25" s="22">
         <v>1</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="24" t="s">
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="17" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="26">
-        <v>0</v>
-      </c>
-      <c r="C26" s="25">
-        <v>0</v>
-      </c>
-      <c r="D26" s="25">
-        <v>0</v>
-      </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-      <c r="F26" s="26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="27">
-        <v>0</v>
-      </c>
-      <c r="H26" s="26">
-        <v>0</v>
-      </c>
-      <c r="I26" s="27">
+      <c r="B26" s="23">
+        <v>1</v>
+      </c>
+      <c r="C26" s="24">
+        <v>1</v>
+      </c>
+      <c r="D26" s="24">
+        <v>1</v>
+      </c>
+      <c r="E26" s="25">
+        <v>1</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0</v>
+      </c>
+      <c r="G26" s="25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0</v>
+      </c>
+      <c r="I26" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:17">
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated CPyU.py to perform load displacement and store.  Need to start implementing pipelines.  Plan to migrate to a preliminary 16-bit architecture once the piped 8-bit is fully operational.  16-bit will be a branch of the 8-bit repo
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="8-bit" sheetId="1" r:id="rId1"/>
+    <sheet name="16-bit" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -446,26 +446,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,7 +764,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -987,15 +987,15 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9" t="s">
@@ -1025,13 +1025,13 @@
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="9" t="s">
@@ -1409,15 +1409,15 @@
       <c r="I21" s="8">
         <v>0</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="9" t="s">
@@ -1447,13 +1447,13 @@
       <c r="I22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="9" t="s">
@@ -1483,13 +1483,13 @@
       <c r="I23" s="8">
         <v>1</v>
       </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">
@@ -1524,16 +1524,16 @@
       <c r="A25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="20">
-        <v>0</v>
-      </c>
-      <c r="C25" s="21">
-        <v>1</v>
-      </c>
-      <c r="D25" s="21">
-        <v>1</v>
-      </c>
-      <c r="E25" s="22">
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20">
+        <v>1</v>
+      </c>
+      <c r="D25" s="20">
+        <v>1</v>
+      </c>
+      <c r="E25" s="21">
         <v>1</v>
       </c>
       <c r="F25" s="16">
@@ -1553,28 +1553,28 @@
       <c r="A26" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="23">
-        <v>1</v>
-      </c>
-      <c r="C26" s="24">
-        <v>1</v>
-      </c>
-      <c r="D26" s="24">
-        <v>1</v>
-      </c>
-      <c r="E26" s="25">
-        <v>1</v>
-      </c>
-      <c r="F26" s="23">
-        <v>0</v>
-      </c>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="25">
+      <c r="B26" s="22">
+        <v>1</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1</v>
+      </c>
+      <c r="D26" s="23">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0</v>
+      </c>
+      <c r="G26" s="24">
+        <v>0</v>
+      </c>
+      <c r="H26" s="22">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added pipeline.py which contains a class for pipelines.  Begin implementation of pipeline structure withn CPyU.py; currently only one pipe exists.  Expansion to five pipelines is next on the list.  After that, incremental updates in terms of opcode functionality will be addressed
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>Op-code</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>br</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>call</t>
@@ -764,7 +761,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -822,16 +819,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -851,16 +848,16 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -880,10 +877,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
@@ -892,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -912,10 +909,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -924,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -944,10 +941,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
@@ -956,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -976,19 +973,19 @@
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
@@ -1014,13 +1011,13 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
       </c>
       <c r="I8" s="8">
         <v>0</v>
@@ -1050,16 +1047,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1079,16 +1076,16 @@
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1108,16 +1105,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1137,16 +1134,16 @@
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1166,16 +1163,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1195,16 +1192,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1224,16 +1221,16 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1253,16 +1250,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1282,10 +1279,10 @@
         <v>1</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="7">
         <v>0</v>
@@ -1311,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -1340,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
@@ -1369,10 +1366,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H20" s="7">
         <v>1</v>
@@ -1410,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -1436,16 +1433,16 @@
         <v>0</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="I22" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="11">
         <v>1</v>
@@ -1493,7 +1490,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="11">
         <v>0</v>
@@ -1511,18 +1508,18 @@
         <v>0</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -1540,18 +1537,18 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="22">
         <v>1</v>
@@ -1580,12 +1577,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="E29" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="D30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added shift, not, cpy and swap to CPyU.py and Assembler.py.  Added in flags and flag control for C, V and N
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
   <si>
     <t>Op-code</t>
   </si>
@@ -174,12 +174,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -397,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -461,6 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -761,7 +768,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -803,7 +810,7 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11">
@@ -832,7 +839,7 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11">
@@ -893,7 +900,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="11">
@@ -984,15 +991,15 @@
       <c r="I7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9" t="s">
@@ -1022,16 +1029,16 @@
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="11">
@@ -1060,7 +1067,7 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="11">
@@ -1089,7 +1096,7 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="11">
@@ -1176,7 +1183,7 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="11">
@@ -1197,11 +1204,11 @@
       <c r="G14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>33</v>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1263,7 +1270,7 @@
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="11">
@@ -1292,7 +1299,7 @@
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="11">
@@ -1321,7 +1328,7 @@
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="11">
@@ -1350,7 +1357,7 @@
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="11">
@@ -1406,15 +1413,15 @@
       <c r="I21" s="8">
         <v>0</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="K21" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="9" t="s">
@@ -1444,13 +1451,13 @@
       <c r="I22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="9" t="s">
@@ -1480,13 +1487,13 @@
       <c r="I23" s="8">
         <v>1</v>
       </c>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">

</xml_diff>

<commit_message>
Added MA pipe for memory write/read.  Added support of Load Displace and Store commands (in both CPyU.py and Assembler.py.  Need to start writing a more comprehensive user guide for programming to guarantee usability beyond just myself.  Also desperately need to add in comments most of the code, very few comments at this point which is starting to become a problem
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
   <si>
     <t>Op-code</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>ld</t>
-  </si>
-  <si>
-    <t>ld (immediate)</t>
   </si>
   <si>
     <t>st</t>
@@ -768,7 +765,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -826,16 +823,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -855,21 +852,21 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="9" t="s">
-        <v>12</v>
+      <c r="A4" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -884,10 +881,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
@@ -896,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -916,10 +913,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -928,12 +925,12 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="9" t="s">
-        <v>13</v>
+      <c r="A6" s="25" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
@@ -948,10 +945,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="7">
         <v>1</v>
@@ -960,12 +957,12 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -980,10 +977,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -992,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
@@ -1003,7 +1000,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -1018,10 +1015,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -1039,7 +1036,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -1054,21 +1051,21 @@
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -1083,21 +1080,21 @@
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
@@ -1112,21 +1109,21 @@
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="11">
         <v>1</v>
@@ -1141,21 +1138,21 @@
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="11">
         <v>1</v>
@@ -1170,21 +1167,21 @@
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="11">
         <v>1</v>
@@ -1199,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="7">
         <v>0</v>
@@ -1213,7 +1210,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="11">
         <v>1</v>
@@ -1228,21 +1225,21 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="11">
         <v>1</v>
@@ -1257,21 +1254,21 @@
         <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="11">
         <v>1</v>
@@ -1286,10 +1283,10 @@
         <v>1</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7">
         <v>0</v>
@@ -1300,7 +1297,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="11">
         <v>1</v>
@@ -1315,10 +1312,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -1329,7 +1326,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="11">
         <v>1</v>
@@ -1344,10 +1341,10 @@
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19" s="7">
         <v>1</v>
@@ -1358,7 +1355,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="11">
         <v>1</v>
@@ -1373,10 +1370,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="7">
         <v>1</v>
@@ -1387,7 +1384,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="11">
         <v>1</v>
@@ -1414,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
@@ -1425,7 +1422,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="11">
         <v>1</v>
@@ -1440,16 +1437,16 @@
         <v>0</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="I22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
@@ -1461,7 +1458,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="11">
         <v>1</v>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="11">
         <v>0</v>
@@ -1515,18 +1512,18 @@
         <v>0</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -1544,18 +1541,18 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="22">
         <v>1</v>
@@ -1584,12 +1581,12 @@
     </row>
     <row r="29" spans="1:17">
       <c r="E29" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="D30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in/out commands.  Moved asm code to asm folder.  Added pcc.bat which just calls Assembler.py.  Bug found when asm file contains underscore.  Currently just throws error prompting user to change filename.  Will be properly handled in the future.
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -765,7 +765,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,7 +961,7 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="11">
@@ -999,7 +999,7 @@
       <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="11">

</xml_diff>